<commit_message>
reverted back to normal
</commit_message>
<xml_diff>
--- a/upload-dir/test.xlsx
+++ b/upload-dir/test.xlsx
@@ -363,8 +363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5537"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,7 +391,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>454876548</v>
+        <v>454876547</v>
       </c>
       <c r="B3" s="2">
         <v>1896.2</v>
@@ -399,7 +399,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>454876549</v>
+        <v>454876547</v>
       </c>
       <c r="B4" s="2">
         <v>992.5</v>
@@ -407,7 +407,7 @@
     </row>
     <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>454876550</v>
+        <v>454876547</v>
       </c>
       <c r="B5" s="2">
         <v>99.25</v>
@@ -415,7 +415,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>454876551</v>
+        <v>454876547</v>
       </c>
       <c r="B6" s="2">
         <v>297.75</v>
@@ -423,7 +423,7 @@
     </row>
     <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>454876552</v>
+        <v>454876547</v>
       </c>
       <c r="B7" s="2">
         <v>1996</v>
@@ -431,7 +431,7 @@
     </row>
     <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>454876553</v>
+        <v>454876547</v>
       </c>
       <c r="B8" s="2">
         <v>9131</v>
@@ -439,7 +439,7 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>454876554</v>
+        <v>454876547</v>
       </c>
       <c r="B9" s="2">
         <v>3093.8</v>
@@ -447,7 +447,7 @@
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>454876555</v>
+        <v>454876547</v>
       </c>
       <c r="B10" s="2">
         <v>10179.6</v>
@@ -455,7 +455,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>454876556</v>
+        <v>454876547</v>
       </c>
       <c r="B11" s="2">
         <v>5089.8</v>
@@ -463,7 +463,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>454876557</v>
+        <v>454876547</v>
       </c>
       <c r="B12" s="2">
         <v>4000</v>
@@ -471,7 +471,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>454876558</v>
+        <v>454876547</v>
       </c>
       <c r="B13" s="2">
         <v>11177.6</v>
@@ -479,7 +479,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>454876559</v>
+        <v>454876547</v>
       </c>
       <c r="B14" s="2">
         <v>4962.5</v>
@@ -487,7 +487,7 @@
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
-        <v>454876560</v>
+        <v>454876547</v>
       </c>
       <c r="B15" s="2">
         <v>3225.63</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
-        <v>454876561</v>
+        <v>454876547</v>
       </c>
       <c r="B16" s="2">
         <v>2878.25</v>
@@ -503,7 +503,7 @@
     </row>
     <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>454876562</v>
+        <v>454876547</v>
       </c>
       <c r="B17" s="2">
         <v>2095.8000000000002</v>
@@ -511,7 +511,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>454876563</v>
+        <v>454876547</v>
       </c>
       <c r="B18" s="2">
         <v>5756.5</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>454876564</v>
+        <v>454876547</v>
       </c>
       <c r="B19" s="2">
         <v>5988</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>454876565</v>
+        <v>454876547</v>
       </c>
       <c r="B20" s="2">
         <v>4000</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="21" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>454876566</v>
+        <v>454876547</v>
       </c>
       <c r="B21" s="2">
         <v>15185.25</v>
@@ -543,7 +543,7 @@
     </row>
     <row r="22" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
-        <v>454876567</v>
+        <v>454876547</v>
       </c>
       <c r="B22" s="2">
         <v>9980</v>
@@ -551,7 +551,7 @@
     </row>
     <row r="23" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
-        <v>454876568</v>
+        <v>454876547</v>
       </c>
       <c r="B23" s="2">
         <v>397</v>
@@ -559,7 +559,7 @@
     </row>
     <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
-        <v>454876569</v>
+        <v>454876547</v>
       </c>
       <c r="B24" s="2">
         <v>694.75</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>454876570</v>
+        <v>454876547</v>
       </c>
       <c r="B25" s="2">
         <v>168.72</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="26" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>454876571</v>
+        <v>454876547</v>
       </c>
       <c r="B26" s="2">
         <v>3000</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>454876572</v>
+        <v>454876547</v>
       </c>
       <c r="B27" s="2">
         <v>4962.5</v>
@@ -591,7 +591,7 @@
     </row>
     <row r="28" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
-        <v>454876573</v>
+        <v>454876547</v>
       </c>
       <c r="B28" s="2">
         <v>3000</v>
@@ -599,7 +599,7 @@
     </row>
     <row r="29" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
-        <v>454876574</v>
+        <v>454876547</v>
       </c>
       <c r="B29" s="2">
         <v>367.23</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="30" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
-        <v>454876575</v>
+        <v>454876547</v>
       </c>
       <c r="B30" s="2">
         <v>2095.8000000000002</v>
@@ -615,7 +615,7 @@
     </row>
     <row r="31" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
-        <v>454876576</v>
+        <v>454876547</v>
       </c>
       <c r="B31" s="2">
         <v>4168.5</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="32" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
-        <v>454876577</v>
+        <v>454876547</v>
       </c>
       <c r="B32" s="2">
         <v>998</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="33" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
-        <v>454876578</v>
+        <v>454876547</v>
       </c>
       <c r="B33" s="2">
         <v>0.1</v>
@@ -44670,6 +44670,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:B5537">
+    <sortCondition ref="A2:A5537"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>